<commit_message>
Validaties TPOD1890 TPOD2080 TPOD2090 TPOD2100 TPOD2110 geimplementeerd door Kadaster
Naar aanleiding van volgende bericht van Kadaster Goedemorgen,

We gaan een vijftal nieuwe validaties opnemen in onze logica. De komende
zullen er zeer waarschijnlijk nog meer volgen. Het gaat nu om de
volgende set:

Nieuw:
(TPOD1890) Het OwObject met identificatie {} heeft het type {}, wat niet overeenkomt met het type in de identificatie.
(TPOD2080) Een instructieregel met identificatie {} moet ofwel een "InstructieregelInstrument", ofwel een "InstructieregelTaakuitoefening" hebben.
(TPOD2090) De normwaarden van de norm met identificatie {} hebben niet hetzelfde type waarde; binnen een norm moeten meerdere normwaarden van hetzelfde type zijn: kwalitatief, kwantitatief, of waardeInRegeltekst
(TPOD2100) De norm met identificatie {} heeft een Eenheid, maar heeft geen normwaarden van het type kwantitatief.
(TPOD2110) HetTekstdeel met identificatie {} heeft een locatie maar geen idealisatie.
</commit_message>
<xml_diff>
--- a/Validatiematrix.xlsx
+++ b/Validatiematrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\TPOD\Validatieregels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w.quak\Git\Geonovum\dso-validatiematrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE282799-7044-4987-95BC-785B7BB1F41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726C9A5A-99A8-4419-A0BA-950D7A963B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6765" yWindow="-21165" windowWidth="45855" windowHeight="20565" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Validatieregels" sheetId="14" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5143" uniqueCount="2166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5143" uniqueCount="2171">
   <si>
     <t>Blokkerend</t>
   </si>
@@ -7218,6 +7218,21 @@
   </si>
   <si>
     <t>Bepaalde stappen in het procedureverloop MOGEN hooguit één keer voorkomen.Sommige stappen worden maar één keer gezet in een procedure en kennen dus ook maar één datum waarop ze voltooid zijn. Als blijkt dat de datum niet correct is; kan die via een mutatie van het procedureverloop aangepast worden. De uniciteit van deze stappen is belangrijk omdat de datum ervan nodig is om de relevantie te bepalen van besluiten en/of kennisgevingen erover.</t>
+  </si>
+  <si>
+    <t>Het OwObject met identificatie {} heeft het type {}, wat niet overeenkomt met het type in de identificatie.</t>
+  </si>
+  <si>
+    <t>Een instructieregel met identificatie {} moet ofwel een "InstructieregelInstrument", ofwel een "InstructieregelTaakuitoefening" hebben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De normwaarden van de norm met identificatie {} hebben niet hetzelfde type waarde; binnen een norm moeten meerdere normwaarden van hetzelfde type zijn: kwalitatief, kwantitatief, of waardeInRegeltekst </t>
+  </si>
+  <si>
+    <t>De norm met identificatie {} heeft een Eenheid, maar heeft geen normwaarden van het type kwantitatief.</t>
+  </si>
+  <si>
+    <t>HetTekstdeel met identificatie {} heeft een locatie maar geen idealisatie.</t>
   </si>
 </sst>
 </file>
@@ -8441,12 +8456,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8557A4-2CF5-4E48-BD49-1C23F60C44EA}">
   <dimension ref="A1:K766"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C410" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C714" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="A3" sqref="A3"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C427" sqref="C427"/>
+      <selection pane="bottomRight" activeCell="G725" sqref="G725"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28567,10 +28582,10 @@
         <v>0</v>
       </c>
       <c r="F714" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G714" s="10" t="s">
-        <v>811</v>
+        <v>2166</v>
       </c>
       <c r="H714" s="10"/>
       <c r="I714" s="10"/>
@@ -28783,10 +28798,10 @@
         <v>0</v>
       </c>
       <c r="F722" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G722" s="10" t="s">
-        <v>811</v>
+        <v>2167</v>
       </c>
       <c r="H722" s="10"/>
       <c r="I722" s="10"/>
@@ -28810,10 +28825,10 @@
         <v>0</v>
       </c>
       <c r="F723" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G723" s="10" t="s">
-        <v>811</v>
+        <v>2168</v>
       </c>
       <c r="H723" s="10"/>
       <c r="I723" s="10"/>
@@ -28837,10 +28852,10 @@
         <v>0</v>
       </c>
       <c r="F724" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G724" s="10" t="s">
-        <v>811</v>
+        <v>2169</v>
       </c>
       <c r="H724" s="10"/>
       <c r="I724" s="10"/>
@@ -28864,10 +28879,10 @@
         <v>0</v>
       </c>
       <c r="F725" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G725" s="10" t="s">
-        <v>811</v>
+        <v>2170</v>
       </c>
       <c r="H725" s="10"/>
       <c r="I725" s="10"/>
@@ -30621,21 +30636,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100216A073BBB3FB3429D87D77C40313058" ma:contentTypeVersion="7" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="8cfc1d06a525c7d4ea1098b3952a2226">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="385505e6-e5d7-4f1a-b335-045f4e6272b3" xmlns:ns3="86b5f7f7-2f15-447a-b5f6-1e4312ec3a6d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="67eef51872945492eed3b93ded28523b" ns2:_="" ns3:_="">
     <xsd:import namespace="385505e6-e5d7-4f1a-b335-045f4e6272b3"/>
@@ -30818,32 +30818,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4AEB88-1F93-43C1-A78E-1A3EC40A664E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="aafb19fa-82be-411d-a6df-c75e9235a4ea"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="3dfebdfe-2b22-40ba-8672-9fbc9b4066c4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{430E6B59-185B-464E-889D-EBB334F9461E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD65B255-3494-4F5F-976E-876698EF30C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30860,4 +30850,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{430E6B59-185B-464E-889D-EBB334F9461E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4AEB88-1F93-43C1-A78E-1A3EC40A664E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="aafb19fa-82be-411d-a6df-c75e9235a4ea"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="3dfebdfe-2b22-40ba-8672-9fbc9b4066c4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Typefout gefixed in OZON0351: wijzingen --> wijzigen
</commit_message>
<xml_diff>
--- a/Validatiematrix.xlsx
+++ b/Validatiematrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w.quak\Git\Geonovum\dso-validatiematrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2BD9D9-2011-45BC-A9EE-0985EC9F6DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C4A3CE-4A16-493D-8D8E-22F05397F3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6765" yWindow="-21165" windowWidth="45855" windowHeight="20565" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7214,9 +7214,6 @@
     <t>Wanneer een object wordt beëindigd, dan mag er geen ander object meer naar verwijzen.</t>
   </si>
   <si>
-    <t>Het beëindigen/wijzingen van een object mag niet leiden tot het verwezen van een ander object.</t>
-  </si>
-  <si>
     <t>Bepaalde stappen in het procedureverloop MOGEN hooguit één keer voorkomen.Sommige stappen worden maar één keer gezet in een procedure en kennen dus ook maar één datum waarop ze voltooid zijn. Als blijkt dat de datum niet correct is; kan die via een mutatie van het procedureverloop aangepast worden. De uniciteit van deze stappen is belangrijk omdat de datum ervan nodig is om de relevantie te bepalen van besluiten en/of kennisgevingen erover.</t>
   </si>
   <si>
@@ -7233,6 +7230,9 @@
   </si>
   <si>
     <t>HetTekstdeel met identificatie {} heeft een locatie maar geen idealisatie.</t>
+  </si>
+  <si>
+    <t>Het beëindigen/wijzigen van een object mag niet leiden tot het verwezen van een ander object.</t>
   </si>
 </sst>
 </file>
@@ -8462,7 +8462,7 @@
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="A3" sqref="A3"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F767" sqref="F767"/>
+      <selection pane="bottomRight" activeCell="C768" sqref="C768"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12637,7 +12637,7 @@
       <c r="J146" s="19"/>
       <c r="K146" s="19"/>
     </row>
-    <row r="147" spans="1:11" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="18">
         <v>2</v>
       </c>
@@ -12664,7 +12664,7 @@
       <c r="J147" s="19"/>
       <c r="K147" s="19"/>
     </row>
-    <row r="148" spans="1:11" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="18">
         <v>2</v>
       </c>
@@ -12691,7 +12691,7 @@
       <c r="J148" s="19"/>
       <c r="K148" s="19"/>
     </row>
-    <row r="149" spans="1:11" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="18">
         <v>2</v>
       </c>
@@ -12718,7 +12718,7 @@
       <c r="J149" s="19"/>
       <c r="K149" s="19"/>
     </row>
-    <row r="150" spans="1:11" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="18">
         <v>2</v>
       </c>
@@ -12747,7 +12747,7 @@
       <c r="J150" s="19"/>
       <c r="K150" s="19"/>
     </row>
-    <row r="151" spans="1:11" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="18">
         <v>2</v>
       </c>
@@ -12778,7 +12778,7 @@
       <c r="J151" s="19"/>
       <c r="K151" s="19"/>
     </row>
-    <row r="152" spans="1:11" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="18">
         <v>2</v>
       </c>
@@ -12805,7 +12805,7 @@
       <c r="J152" s="19"/>
       <c r="K152" s="19"/>
     </row>
-    <row r="153" spans="1:11" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="18">
         <v>2</v>
       </c>
@@ -12832,7 +12832,7 @@
       <c r="J153" s="19"/>
       <c r="K153" s="19"/>
     </row>
-    <row r="154" spans="1:11" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="18">
         <v>2</v>
       </c>
@@ -16332,7 +16332,7 @@
       <c r="J279" s="17"/>
       <c r="K279" s="17"/>
     </row>
-    <row r="280" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:11" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A280" s="12">
         <v>8</v>
       </c>
@@ -19302,7 +19302,7 @@
       <c r="J389" s="17"/>
       <c r="K389" s="17"/>
     </row>
-    <row r="390" spans="1:11" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A390" s="12">
         <v>8</v>
       </c>
@@ -19310,7 +19310,7 @@
         <v>765</v>
       </c>
       <c r="C390" s="10" t="s">
-        <v>2164</v>
+        <v>2170</v>
       </c>
       <c r="D390" s="10" t="s">
         <v>260</v>
@@ -20409,7 +20409,7 @@
       <c r="J430" s="10"/>
       <c r="K430" s="10"/>
     </row>
-    <row r="431" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:11" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A431" s="12">
         <v>8</v>
       </c>
@@ -20947,7 +20947,7 @@
       <c r="J448" s="19"/>
       <c r="K448" s="19"/>
     </row>
-    <row r="449" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:11" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A449" s="18">
         <v>2</v>
       </c>
@@ -24101,7 +24101,7 @@
         <v>1015</v>
       </c>
       <c r="C555" s="19" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="D555" s="18" t="s">
         <v>1481</v>
@@ -28586,7 +28586,7 @@
         <v>2</v>
       </c>
       <c r="G714" s="10" t="s">
-        <v>2166</v>
+        <v>2165</v>
       </c>
       <c r="H714" s="10"/>
       <c r="I714" s="10"/>
@@ -28802,7 +28802,7 @@
         <v>2</v>
       </c>
       <c r="G722" s="10" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="H722" s="10"/>
       <c r="I722" s="10"/>
@@ -28829,7 +28829,7 @@
         <v>2</v>
       </c>
       <c r="G723" s="10" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="H723" s="10"/>
       <c r="I723" s="10"/>
@@ -28856,7 +28856,7 @@
         <v>2</v>
       </c>
       <c r="G724" s="10" t="s">
-        <v>2169</v>
+        <v>2168</v>
       </c>
       <c r="H724" s="10"/>
       <c r="I724" s="10"/>
@@ -28883,7 +28883,7 @@
         <v>2</v>
       </c>
       <c r="G725" s="10" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="H725" s="10"/>
       <c r="I725" s="10"/>
@@ -30001,9 +30001,15 @@
   <autoFilter ref="A1:K766" xr:uid="{6D8557A4-2CF5-4E48-BD49-1C23F60C44EA}">
     <filterColumn colId="1">
       <filters>
-        <filter val="OZON0021"/>
-        <filter val="RTRG0021"/>
-        <filter val="STOP0021"/>
+        <filter val="LVBB3510"/>
+        <filter val="LVBB3511"/>
+        <filter val="LVBB3512"/>
+        <filter val="LVBB3513"/>
+        <filter val="LVBB3514"/>
+        <filter val="LVBB3515"/>
+        <filter val="LVBB3516"/>
+        <filter val="LVBB3517"/>
+        <filter val="OZON0351"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K766">
@@ -30827,18 +30833,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -30861,6 +30867,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{430E6B59-185B-464E-889D-EBB334F9461E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4AEB88-1F93-43C1-A78E-1A3EC40A664E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="aafb19fa-82be-411d-a6df-c75e9235a4ea"/>
@@ -30875,12 +30889,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{430E6B59-185B-464E-889D-EBB334F9461E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
redactioneel een logo aangepast.
</commit_message>
<xml_diff>
--- a/Validatiematrix.xlsx
+++ b/Validatiematrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w.quak\Git\Geonovum\dso-validatiematrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18724A87-3279-45A7-893D-7F5B9B138862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471B24B8-EBB9-4DB1-B5A2-E771E0958DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12405" yWindow="-21555" windowWidth="22980" windowHeight="12195" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16320" yWindow="-20655" windowWidth="22980" windowHeight="12195" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Validatieregels" sheetId="14" r:id="rId1"/>
@@ -7256,13 +7256,13 @@
     <t>Intrekken-vervangen (scenario 0) mag niet worden gebruikt in combinatie met meerdere regelingen.</t>
   </si>
   <si>
-    <t>Iedere verwijzing naar een gmlObject vanuit een Lijn moet verwijzen naar een object van type GM_LineString of GM_MultiLinestring  GM_MultiLinestring.</t>
-  </si>
-  <si>
     <t>Iedere verwijzing naar een gmlObject vanuit een Punt moet verwijzen naar een object van type GM_Point of GM_MultiPoint.</t>
   </si>
   <si>
     <t>Iedere verwijzing naar een gmlObject vanuit een Gebied moet verwijzen naar een object van type GM_Surface of GM_MultiSurface.</t>
+  </si>
+  <si>
+    <t>Iedere verwijzing naar een gmlObject vanuit een Lijn moet verwijzen naar een object van type GM_LineString of GM_MultiLinestring.</t>
   </si>
 </sst>
 </file>
@@ -7429,7 +7429,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -7491,6 +7491,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -8482,7 +8485,7 @@
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="A3" sqref="A3"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C724" sqref="C724"/>
+      <selection pane="bottomRight" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -20299,7 +20302,7 @@
       <c r="B426" s="9" t="s">
         <v>2168</v>
       </c>
-      <c r="C426" t="s">
+      <c r="C426" s="21" t="s">
         <v>2169</v>
       </c>
       <c r="D426" s="9"/>
@@ -20316,7 +20319,7 @@
       <c r="B427" s="9" t="s">
         <v>2170</v>
       </c>
-      <c r="C427" t="s">
+      <c r="C427" s="21" t="s">
         <v>2174</v>
       </c>
       <c r="D427" s="9"/>
@@ -20333,7 +20336,7 @@
       <c r="B428" s="9" t="s">
         <v>2171</v>
       </c>
-      <c r="C428" t="s">
+      <c r="C428" s="21" t="s">
         <v>2175</v>
       </c>
       <c r="D428" s="9"/>
@@ -20350,7 +20353,7 @@
       <c r="B429" s="9" t="s">
         <v>2172</v>
       </c>
-      <c r="C429" t="s">
+      <c r="C429" s="21" t="s">
         <v>2176</v>
       </c>
       <c r="D429" s="9"/>
@@ -20367,7 +20370,7 @@
       <c r="B430" s="9" t="s">
         <v>2173</v>
       </c>
-      <c r="C430" t="s">
+      <c r="C430" s="21" t="s">
         <v>2177</v>
       </c>
       <c r="D430" s="9"/>
@@ -28706,7 +28709,7 @@
         <v>143</v>
       </c>
       <c r="C720" s="9" t="s">
-        <v>2178</v>
+        <v>2180</v>
       </c>
       <c r="D720" s="9" t="s">
         <v>257</v>
@@ -28733,7 +28736,7 @@
         <v>144</v>
       </c>
       <c r="C721" s="9" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="D721" s="9" t="s">
         <v>257</v>
@@ -28760,7 +28763,7 @@
         <v>145</v>
       </c>
       <c r="C722" s="9" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
       <c r="D722" s="9" t="s">
         <v>257</v>
@@ -30920,18 +30923,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -30954,14 +30957,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{430E6B59-185B-464E-889D-EBB334F9461E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4AEB88-1F93-43C1-A78E-1A3EC40A664E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="aafb19fa-82be-411d-a6df-c75e9235a4ea"/>
@@ -30976,4 +30971,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{430E6B59-185B-464E-889D-EBB334F9461E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>